<commit_message>
cleanup code a bit
</commit_message>
<xml_diff>
--- a/Data Sources.xlsx
+++ b/Data Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\Final_Project\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D381FB-F640-497D-AD05-A38D472C69C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE68368-A0DE-451D-8BE7-4D570E5AB1BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{34B7DB9E-386B-4267-B34D-AB0C4C1D17F6}"/>
   </bookViews>
@@ -1555,7 +1555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5874C8D2-4F1D-481B-B1B7-FE0CAA1DBFC4}">
   <dimension ref="A1:A65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>

</xml_diff>

<commit_message>
8 Datasources in Database
</commit_message>
<xml_diff>
--- a/Data Sources.xlsx
+++ b/Data Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\Final_Project\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE68368-A0DE-451D-8BE7-4D570E5AB1BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB51B22A-1CCC-436D-BAD0-3C4B41ACD1D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{34B7DB9E-386B-4267-B34D-AB0C4C1D17F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{34B7DB9E-386B-4267-B34D-AB0C4C1D17F6}"/>
   </bookViews>
   <sheets>
     <sheet name="State_Level_Summary" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">State_Level_Summary!$A$3:$B$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="131">
   <si>
     <t>Credit Source (1Point3Acres COVID-19 Data Access Application) when using their data</t>
   </si>
@@ -430,6 +431,12 @@
   </si>
   <si>
     <t>kaggle datasets download -d sudalairajkumar/covid19-in-usa</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/sudalairajkumar/covid19-in-usa/download</t>
+  </si>
+  <si>
+    <t>'https://www.kaggle.com/sudalairajkumar/novel-corona-virus-2019-dataset#COVID19_line_list_data.csv</t>
   </si>
 </sst>
 </file>
@@ -1362,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB690ADC-8B73-4964-8C87-D8CF3B15A9C8}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1374,77 +1381,83 @@
     <col min="2" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:2">
       <c r="A9" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:2">
       <c r="A11" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:2">
       <c r="A12" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:2">
       <c r="A13" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:2">
       <c r="A14" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:2">
       <c r="A15" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:2">
       <c r="A16" s="7" t="s">
         <v>120</v>
       </c>
@@ -1467,6 +1480,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="us_states_covid19_daily.csv" xr:uid="{70E17B6A-985B-47DE-9A32-F8D68BFA24AC}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{950435BD-7E51-4627-B13E-A343E010EE62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1555,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5874C8D2-4F1D-481B-B1B7-FE0CAA1DBFC4}">
   <dimension ref="A1:A65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="148" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>